<commit_message>
Cards created from CSV tings
</commit_message>
<xml_diff>
--- a/Documents/WSOA3004_ExamGame_Cards.xlsx
+++ b/Documents/WSOA3004_ExamGame_Cards.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wits\Game Design\Unity Projects\GitHub\DungeonDeckBuilder\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D863E0-A824-447F-8513-04745C196890}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345E625F-3123-4059-9AA9-DD8EFBD6CF7E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7344" windowHeight="5652" xr2:uid="{8A751AE2-55CF-47D2-91C1-ECB4D3596336}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7344" windowHeight="5652" xr2:uid="{8A751AE2-55CF-47D2-91C1-ECB4D3596336}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,20 +532,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590467C9-99E5-4BCA-A11E-6CA274D3463F}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -553,258 +557,258 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-2</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -821,19 +825,19 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -841,144 +845,144 @@
         <v>36</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -989,10 +993,8 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1000,10 +1002,8 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1011,10 +1011,8 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1022,8 +1020,6 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>